<commit_message>
Limit lite roads to motorway/A-road profile and expand import template dataset
</commit_message>
<xml_diff>
--- a/data/example import.xlsx
+++ b/data/example import.xlsx
@@ -438,79 +438,80 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="36" customWidth="1" min="1" max="1"/>
+    <col width="28" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="14" customWidth="1" min="3" max="3"/>
-    <col width="40" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="42" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="28" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="42" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="26" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="34" customWidth="1" min="10" max="10"/>
     <col width="10" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Entity Type</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>DOB</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Postcode</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Latitude</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Longitude</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Target</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Relationship</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>i2_type</t>
         </is>
@@ -519,7 +520,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Andy JONES DOB 01/01/2000</t>
+          <t>Andy JONES</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -527,7 +528,11 @@
           <t>Person</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>01/01/2000</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>1 Osmond Drive, Wells, Somerset</t>
@@ -552,7 +557,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Subject linked to logistics firm</t>
+          <t>Primary subject</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -564,225 +569,765 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ACME Logistics Ltd</t>
+          <t>Sarah PATEL</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Organisation</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>14/08/1987</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1 Canada Square, London</t>
+          <t>Flat 2, 18 Broad Street, Bristol</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>E14 5AB</t>
+          <t>BS1 2HG</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>North Dock Warehouse</t>
+          <t>ACME Logistics Ltd</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Owns/Uses</t>
+          <t>Director/Officer</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Commercial logistics footprint</t>
+          <t>Officer linkage</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>ET4</t>
+          <t>ET5</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>North Dock Warehouse</t>
+          <t>Danny KENT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Location</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>23/03/1983</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>North Dock Road, London</t>
+          <t>Terminal 3, Manchester Airport</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>E16 2GT</t>
+          <t>M90 1QX</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Andy JONES</t>
+          <t>KLM1142</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Visited</t>
+          <t>Passenger</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Known meeting location</t>
+          <t>Travel association</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>ET1</t>
+          <t>ET5</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>KLM1142</t>
+          <t>Paul SHARP</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Communication</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>51.4700</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>-0.4543</t>
-        </is>
-      </c>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>11/11/1979</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Regent's Park, London</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>NW1 4NR</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Andy JONES</t>
+          <t>North Dock Warehouse</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Linked Flight</t>
+          <t>Visited</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Flight reference observed in comms</t>
+          <t>Seen at location</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>ET8</t>
+          <t>ET5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sarah PATEL DOB 14/08/1987</t>
+          <t>ACME Logistics Ltd</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Flat 2, 18 Broad Street, Bristol</t>
+          <t>1 Canada Square, London</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>BS1 2HG</t>
+          <t>E14 5AB</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>ACME Logistics Ltd</t>
+          <t>North Dock Warehouse</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Director/Officer</t>
+          <t>Owns/Uses</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Officer linkage from CH records</t>
+          <t>UK logistics business</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>ET5</t>
+          <t>ET4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ZX-991122</t>
+          <t>Moonshadow Marine Ltd</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Vehicle</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Birmingham</t>
+          <t>Quayside House, Liverpool</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>B1 1AA</t>
+          <t>L3 1BP</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
+          <t>Moonshadow</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Operates</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Maritime operator</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>ET4</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>North Dock Warehouse</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>North Dock Road, London</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>E16 2GT</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Andy JONES</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Meeting Location</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Regular meetup site</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>ET1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>500 Silver Street, Greensville</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>500 Silver Street, Greensville</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>SW1A 1AA</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Sarah PATEL</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Residence</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Address from chart</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>ET1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>KLM1142</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Communication</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>51.47</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-0.4543</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Manchester Airport (MAN)</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Route</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Flight identifier</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>ET8</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BAW23T</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Communication</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>50.939</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-1.404</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>CULDROSE (EGDR)</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Destination</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Ops-linked flight</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>ET8</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ZX-991122</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Vehicle</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Birmingham</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>B1 1AA</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
           <t>ACME Logistics Ltd</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Company Vehicle</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Fleet vehicle marker</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Fleet marker</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>ET3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>AB12CDE</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Vehicle</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Leeds</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LS1 4AP</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Paul SHARP</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Observed With</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Vehicle observation</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>ET3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Moonshadow</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Marigot Bay Marina, Castries</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>13.9697</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-61.0378</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Moonshadow Marine Ltd</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Moored At</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Vessel berth location</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>ET1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Waterfront Bar</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Harbour Front, Castries</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>13.995</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-61.01</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Sam STEELE</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Meeting</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Witness meeting point</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>ET1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Sam STEELE</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>25/02/1984</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Castries, Saint Lucia</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>13.9972</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-61.0068</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Waterfront Bar</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Sighted</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Witness sighting</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>ET5</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>NCA-REF-2026-001</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Communication</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Andy JONES</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Reference</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Case reference handle</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>ET8</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Finance Account 4931-1291</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Organisation</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Town Corp Bank, London</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>EC2M 7PP</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>ACME Logistics Ltd</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Account Holder</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Financial account proxy</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>ET4</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>EGDR - CULDROSE</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>RNAS Culdrose, Helston</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>TR12 7RH</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>BAW23T</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Destination</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Airfield node</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>ET1</t>
         </is>
       </c>
     </row>

</xml_diff>